<commit_message>
test: add model2 from 2020 to 2021
</commit_message>
<xml_diff>
--- a/mlResults/ML Model Metadata.xlsx
+++ b/mlResults/ML Model Metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,30 +451,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Model name</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Parameters</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Model Description</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Model Advantage</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Model Drawback</t>
         </is>
@@ -493,32 +498,35 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Model 1</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Iterative gaussian Imputer</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>n_restarts_optimizer = 10,n_nearest_features=10, initial_strategy='mean', imputation_order='ascending'</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Iterative Imputer with a gaussian process regressor base.</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>We can think of model as quite literally predicting a Gaussian distribution at each test point. Hence,easy to compute prediction interval</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Distributional Assumption, lack of feature importance ranking, does not take the year to year relation into account</t>
         </is>
@@ -537,32 +545,35 @@
       <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Model 2</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Random Forest Regressor</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>n_estimators, maximum depth (tuned via cross-validation), initial_strategy="KNNimputer"</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t xml:space="preserve">A random forest is a meta estimator that fits a number of classifying decision trees on various sub-samples of the dataset. Run on a year-by-year basis </t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>uses averaging to improve the predictive accuracy and control over-fitting via bootsrapping</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -577,32 +588,35 @@
       <c r="D4" t="n">
         <v>2</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Model 3</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Gradient boost Regressor</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>loss_function, learning_rate, n_estimators, maximum depth (tuned via cross-validation), initial_strategy="KNNimputer"</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>builds an additive model in a forward stage-wise fashion. In each stage a regression tree is fit on the negative gradient of the given loss function. Run on a year-by-year basis</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Higher point estimation accuracy</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Overfitting especially when there is noisy data</t>
         </is>
@@ -621,32 +635,35 @@
       <c r="D5" t="n">
         <v>3</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>Model 4</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Extratree Regressor</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>n_estimators, maximum depth (tuned via cross-validation), initial_strategy="KNNimputer"</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>estimator that fits a number of randomized decision trees (a.k.a. extra-trees) on various sub-samples of the dataset. Run on a year-by-year basis</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>uses averaging to improve the predictive accuracy and control over-fitting via randomization, faster computation</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>challenged by a high number of noisy features (in high dimensional data-sets)</t>
         </is>
@@ -665,82 +682,58 @@
       <c r="D6" t="n">
         <v>4</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Model 5</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>SAITS</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
         <is>
           <t>Self-Attention-based Imputation for Time Series,SAITS learns missing values from a weighted combination of two diagonally-masked self-attention (DMSA) blocks(Trained by a joint-optimization approach)</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Best for Time-series</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
         <is>
           <t>Model 2</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>crossectional random forest</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>run random forest year by year basis</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>crossectional randomforest</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>run random forest model year by year bbasis</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Model 2</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>crossectional randomforest</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>run random forest model year by year</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
test: add model2 from 2019 to 2020
</commit_message>
<xml_diff>
--- a/mlResults/ML Model Metadata.xlsx
+++ b/mlResults/ML Model Metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,30 +456,35 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Model name</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Parameters</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Model Description</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Model Advantage</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Model Drawback</t>
         </is>
@@ -501,32 +506,35 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Model 1</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Iterative gaussian Imputer</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>n_restarts_optimizer = 10,n_nearest_features=10, initial_strategy='mean', imputation_order='ascending'</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Iterative Imputer with a gaussian process regressor base.</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>We can think of model as quite literally predicting a Gaussian distribution at each test point. Hence,easy to compute prediction interval</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Distributional Assumption, lack of feature importance ranking, does not take the year to year relation into account</t>
         </is>
@@ -548,32 +556,35 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Model 2</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Random Forest Regressor</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>n_estimators, maximum depth (tuned via cross-validation), initial_strategy="KNNimputer"</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t xml:space="preserve">A random forest is a meta estimator that fits a number of classifying decision trees on various sub-samples of the dataset. Run on a year-by-year basis </t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>uses averaging to improve the predictive accuracy and control over-fitting via bootsrapping</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -591,32 +602,35 @@
       <c r="E4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>Model 3</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Gradient boost Regressor</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>loss_function, learning_rate, n_estimators, maximum depth (tuned via cross-validation), initial_strategy="KNNimputer"</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>builds an additive model in a forward stage-wise fashion. In each stage a regression tree is fit on the negative gradient of the given loss function. Run on a year-by-year basis</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Higher point estimation accuracy</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Overfitting especially when there is noisy data</t>
         </is>
@@ -638,32 +652,35 @@
       <c r="E5" t="n">
         <v>3</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Model 4</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Extratree Regressor</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>n_estimators, maximum depth (tuned via cross-validation), initial_strategy="KNNimputer"</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>estimator that fits a number of randomized decision trees (a.k.a. extra-trees) on various sub-samples of the dataset. Run on a year-by-year basis</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>uses averaging to improve the predictive accuracy and control over-fitting via randomization, faster computation</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>challenged by a high number of noisy features (in high dimensional data-sets)</t>
         </is>
@@ -685,55 +702,61 @@
       <c r="E6" t="n">
         <v>4</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Model 5</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>SAITS</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Self-Attention-based Imputation for Time Series,SAITS learns missing values from a weighted combination of two diagonally-masked self-attention (DMSA) blocks(Trained by a joint-optimization approach)</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Best for Time-series</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t>Model 2</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>crossectional randomforest</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
         <is>
           <t>run random forest model year by year bbasis</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>